<commit_message>
Schema changed and turn method finished (failed)
</commit_message>
<xml_diff>
--- a/bin/com/martdel/rubik/schema.xlsx
+++ b/bin/com/martdel/rubik/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartDel\Desktop\programmation\Java\rubik\src\com\martdel\rubik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D32B3C13-503D-4F7C-98BE-B02FC79CE477}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353B810F-8796-478A-AF19-FE128A91F543}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="24240" windowHeight="13140" xr2:uid="{B117DAF9-EA99-4BEA-8465-1CDD5ECE0916}"/>
   </bookViews>
@@ -360,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -580,6 +580,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -899,7 +908,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,13 +937,13 @@
       <c r="G2" s="6"/>
       <c r="H2" s="2"/>
       <c r="I2" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J2" s="7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K2" s="7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L2" s="5"/>
     </row>
@@ -1053,13 +1062,13 @@
       <c r="G6" s="6"/>
       <c r="H6" s="12"/>
       <c r="I6" s="15">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J6" s="15">
         <v>7</v>
       </c>
       <c r="K6" s="15">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L6" s="14"/>
     </row>
@@ -1095,10 +1104,10 @@
         <v>1</v>
       </c>
       <c r="J8" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K8" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L8" s="5"/>
     </row>
@@ -1217,13 +1226,13 @@
       <c r="G12" s="6"/>
       <c r="H12" s="12"/>
       <c r="I12" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J12" s="15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K12" s="15">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L12" s="14"/>
     </row>
@@ -1283,8 +1292,8 @@
         <v>3</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="8">
-        <v>1</v>
+      <c r="H15" s="76">
+        <v>8</v>
       </c>
       <c r="I15" s="65">
         <v>1</v>
@@ -1295,8 +1304,8 @@
       <c r="K15" s="67">
         <v>3</v>
       </c>
-      <c r="L15" s="74">
-        <v>8</v>
+      <c r="L15" s="75">
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1316,8 +1325,8 @@
         <v>5</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="10">
-        <v>2</v>
+      <c r="H16" s="77">
+        <v>7</v>
       </c>
       <c r="I16" s="68">
         <v>4</v>
@@ -1328,7 +1337,7 @@
       <c r="K16" s="70">
         <v>5</v>
       </c>
-      <c r="L16" s="74">
+      <c r="L16" s="75">
         <v>7</v>
       </c>
     </row>
@@ -1349,8 +1358,8 @@
         <v>8</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="10">
-        <v>3</v>
+      <c r="H17" s="77">
+        <v>6</v>
       </c>
       <c r="I17" s="71">
         <v>6</v>
@@ -1361,33 +1370,33 @@
       <c r="K17" s="73">
         <v>8</v>
       </c>
-      <c r="L17" s="74">
-        <v>6</v>
+      <c r="L17" s="75">
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="12"/>
       <c r="C18" s="15">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D18" s="15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E18" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="6"/>
       <c r="H18" s="12"/>
       <c r="I18" s="13">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J18" s="13">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K18" s="13">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L18" s="14"/>
     </row>

</xml_diff>

<commit_message>
Bug in the method turnFaceRight fixed (but not test)
</commit_message>
<xml_diff>
--- a/bin/com/martdel/rubik/schema.xlsx
+++ b/bin/com/martdel/rubik/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartDel\Desktop\programmation\Java\rubik\src\com\martdel\rubik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353B810F-8796-478A-AF19-FE128A91F543}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D902E3-A5D5-4739-BB7A-5091EC42E03C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="24240" windowHeight="13140" xr2:uid="{B117DAF9-EA99-4BEA-8465-1CDD5ECE0916}"/>
   </bookViews>
@@ -117,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -356,11 +356,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -444,27 +470,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -590,6 +607,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -908,7 +937,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,20 +989,20 @@
       <c r="E3" s="22">
         <v>3</v>
       </c>
-      <c r="F3" s="74">
+      <c r="F3" s="71">
         <v>3</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="10">
         <v>3</v>
       </c>
-      <c r="I3" s="47">
-        <v>1</v>
-      </c>
-      <c r="J3" s="48">
+      <c r="I3" s="44">
+        <v>1</v>
+      </c>
+      <c r="J3" s="45">
         <v>2</v>
       </c>
-      <c r="K3" s="49">
+      <c r="K3" s="46">
         <v>3</v>
       </c>
       <c r="L3" s="11">
@@ -993,20 +1022,20 @@
       <c r="E4" s="25">
         <v>5</v>
       </c>
-      <c r="F4" s="74">
+      <c r="F4" s="71">
         <v>2</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="10">
         <v>5</v>
       </c>
-      <c r="I4" s="50">
+      <c r="I4" s="47">
         <v>4</v>
       </c>
-      <c r="J4" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="52">
+      <c r="J4" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="49">
         <v>5</v>
       </c>
       <c r="L4" s="11">
@@ -1026,20 +1055,20 @@
       <c r="E5" s="28">
         <v>8</v>
       </c>
-      <c r="F5" s="74">
+      <c r="F5" s="71">
         <v>1</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="10">
         <v>8</v>
       </c>
-      <c r="I5" s="53">
-        <v>6</v>
-      </c>
-      <c r="J5" s="54">
+      <c r="I5" s="50">
+        <v>6</v>
+      </c>
+      <c r="J5" s="51">
         <v>7</v>
       </c>
-      <c r="K5" s="55">
+      <c r="K5" s="52">
         <v>8</v>
       </c>
       <c r="L5" s="11">
@@ -1112,32 +1141,32 @@
       <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="10">
-        <v>1</v>
-      </c>
-      <c r="C9" s="29">
-        <v>1</v>
-      </c>
-      <c r="D9" s="30">
+      <c r="B9" s="78">
+        <v>3</v>
+      </c>
+      <c r="C9" s="75">
+        <v>1</v>
+      </c>
+      <c r="D9" s="29">
         <v>2</v>
       </c>
-      <c r="E9" s="31">
-        <v>3</v>
-      </c>
-      <c r="F9" s="11">
-        <v>3</v>
+      <c r="E9" s="30">
+        <v>3</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="16">
-        <v>1</v>
-      </c>
-      <c r="I9" s="56">
-        <v>1</v>
-      </c>
-      <c r="J9" s="57">
+        <v>3</v>
+      </c>
+      <c r="I9" s="53">
+        <v>1</v>
+      </c>
+      <c r="J9" s="54">
         <v>2</v>
       </c>
-      <c r="K9" s="58">
+      <c r="K9" s="55">
         <v>3</v>
       </c>
       <c r="L9" s="17">
@@ -1145,32 +1174,32 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="10">
+      <c r="B10" s="78">
+        <v>5</v>
+      </c>
+      <c r="C10" s="76">
         <v>4</v>
       </c>
-      <c r="C10" s="32">
+      <c r="D10" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="32">
+        <v>5</v>
+      </c>
+      <c r="F10" s="10">
         <v>4</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="34">
-        <v>5</v>
-      </c>
-      <c r="F10" s="11">
-        <v>5</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="16">
+        <v>5</v>
+      </c>
+      <c r="I10" s="56">
         <v>4</v>
       </c>
-      <c r="I10" s="59">
+      <c r="J10" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="K10" s="61">
+      <c r="K10" s="58">
         <v>5</v>
       </c>
       <c r="L10" s="17">
@@ -1178,32 +1207,32 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10">
-        <v>6</v>
-      </c>
-      <c r="C11" s="35">
-        <v>6</v>
-      </c>
-      <c r="D11" s="36">
+      <c r="B11" s="78">
+        <v>8</v>
+      </c>
+      <c r="C11" s="77">
+        <v>6</v>
+      </c>
+      <c r="D11" s="33">
         <v>7</v>
       </c>
-      <c r="E11" s="37">
-        <v>8</v>
-      </c>
-      <c r="F11" s="11">
-        <v>8</v>
+      <c r="E11" s="34">
+        <v>8</v>
+      </c>
+      <c r="F11" s="10">
+        <v>6</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="16">
-        <v>6</v>
-      </c>
-      <c r="I11" s="62">
-        <v>6</v>
-      </c>
-      <c r="J11" s="63">
+        <v>8</v>
+      </c>
+      <c r="I11" s="59">
+        <v>6</v>
+      </c>
+      <c r="J11" s="60">
         <v>7</v>
       </c>
-      <c r="K11" s="64">
+      <c r="K11" s="61">
         <v>8</v>
       </c>
       <c r="L11" s="17">
@@ -1279,32 +1308,32 @@
       <c r="B15" s="18">
         <v>3</v>
       </c>
-      <c r="C15" s="38">
-        <v>1</v>
-      </c>
-      <c r="D15" s="39">
+      <c r="C15" s="35">
+        <v>1</v>
+      </c>
+      <c r="D15" s="36">
         <v>2</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="37">
         <v>3</v>
       </c>
       <c r="F15" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="76">
-        <v>8</v>
-      </c>
-      <c r="I15" s="65">
-        <v>1</v>
-      </c>
-      <c r="J15" s="66">
+      <c r="H15" s="73">
+        <v>8</v>
+      </c>
+      <c r="I15" s="62">
+        <v>1</v>
+      </c>
+      <c r="J15" s="63">
         <v>2</v>
       </c>
-      <c r="K15" s="67">
-        <v>3</v>
-      </c>
-      <c r="L15" s="75">
+      <c r="K15" s="64">
+        <v>3</v>
+      </c>
+      <c r="L15" s="72">
         <v>6</v>
       </c>
     </row>
@@ -1312,32 +1341,32 @@
       <c r="B16" s="18">
         <v>5</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="38">
         <v>4</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="40">
         <v>5</v>
       </c>
       <c r="F16" s="19">
+        <v>4</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="74">
+        <v>7</v>
+      </c>
+      <c r="I16" s="65">
+        <v>4</v>
+      </c>
+      <c r="J16" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="77">
-        <v>7</v>
-      </c>
-      <c r="I16" s="68">
-        <v>4</v>
-      </c>
-      <c r="J16" s="69" t="s">
+      <c r="K16" s="67">
         <v>5</v>
       </c>
-      <c r="K16" s="70">
-        <v>5</v>
-      </c>
-      <c r="L16" s="75">
+      <c r="L16" s="72">
         <v>7</v>
       </c>
     </row>
@@ -1345,32 +1374,32 @@
       <c r="B17" s="18">
         <v>8</v>
       </c>
-      <c r="C17" s="44">
-        <v>6</v>
-      </c>
-      <c r="D17" s="45">
+      <c r="C17" s="41">
+        <v>6</v>
+      </c>
+      <c r="D17" s="42">
         <v>7</v>
       </c>
-      <c r="E17" s="46">
+      <c r="E17" s="43">
         <v>8</v>
       </c>
       <c r="F17" s="19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="77">
-        <v>6</v>
-      </c>
-      <c r="I17" s="71">
-        <v>6</v>
-      </c>
-      <c r="J17" s="72">
+      <c r="H17" s="74">
+        <v>6</v>
+      </c>
+      <c r="I17" s="68">
+        <v>6</v>
+      </c>
+      <c r="J17" s="69">
         <v>7</v>
       </c>
-      <c r="K17" s="73">
-        <v>8</v>
-      </c>
-      <c r="L17" s="75">
+      <c r="K17" s="70">
+        <v>8</v>
+      </c>
+      <c r="L17" s="72">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Functions for turning faces done and finished + test those functions (methods) : turnFaceLeft and turnFaceRight
</commit_message>
<xml_diff>
--- a/bin/com/martdel/rubik/schema.xlsx
+++ b/bin/com/martdel/rubik/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartDel\Desktop\programmation\Java\rubik\src\com\martdel\rubik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D902E3-A5D5-4739-BB7A-5091EC42E03C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B10133-6B3E-499F-B56A-CFD9FBDDFFD3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="24240" windowHeight="13140" xr2:uid="{B117DAF9-EA99-4BEA-8465-1CDD5ECE0916}"/>
   </bookViews>
@@ -937,7 +937,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,13 +954,13 @@
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" s="4">
         <v>2</v>
       </c>
       <c r="E2" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="6"/>
@@ -1118,13 +1118,13 @@
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" s="7">
         <v>2</v>
       </c>
       <c r="E8" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="6"/>
@@ -1282,13 +1282,13 @@
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D14" s="7">
         <v>5</v>
       </c>
       <c r="E14" s="7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>

</xml_diff>